<commit_message>
Final Edit of file; transfered times over
Everything should be good!!
</commit_message>
<xml_diff>
--- a/BeSmoke Planner1.xlsx
+++ b/BeSmoke Planner1.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18326"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UM\Documents\GitHub\besmoke\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\OneDrive\Documents\GitHub\besmoke\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="13" documentId="2A840FD9468AD540D7E421D158C0C57B14D0C799" xr6:coauthVersionLast="21" xr6:coauthVersionMax="21" xr10:uidLastSave="{0424E299-5560-4EC6-BA2D-0E8CD26D84B6}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9516"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -155,7 +156,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -498,6 +499,9 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="11">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -531,29 +535,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="19">
-    <cellStyle name="% complete" xfId="16"/>
-    <cellStyle name="% complete (beyond plan) legend" xfId="18"/>
-    <cellStyle name="Activity" xfId="2"/>
-    <cellStyle name="Actual (beyond plan) legend" xfId="17"/>
-    <cellStyle name="Actual legend" xfId="15"/>
+    <cellStyle name="% complete" xfId="16" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="% complete (beyond plan) legend" xfId="18" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Activity" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Actual (beyond plan) legend" xfId="17" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Actual legend" xfId="15" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
     <cellStyle name="Explanatory Text" xfId="12" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="9" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="10" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="11" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Label" xfId="5"/>
+    <cellStyle name="Label" xfId="5" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Percent Complete" xfId="6"/>
-    <cellStyle name="Period Headers" xfId="3"/>
-    <cellStyle name="Period Highlight Control" xfId="7"/>
-    <cellStyle name="Period Value" xfId="13"/>
-    <cellStyle name="Plan legend" xfId="14"/>
-    <cellStyle name="Project Headers" xfId="4"/>
+    <cellStyle name="Percent Complete" xfId="6" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="Period Headers" xfId="3" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="Period Highlight Control" xfId="7" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="Period Value" xfId="13" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="Plan legend" xfId="14" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="Project Headers" xfId="4" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
     <cellStyle name="Title" xfId="8" builtinId="15" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="10">
@@ -713,14 +714,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="B10:F15" totalsRowShown="0">
-  <autoFilter ref="B10:F15"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table4" displayName="Table4" ref="B10:F15" totalsRowShown="0">
+  <autoFilter ref="B10:F15" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Person"/>
-    <tableColumn id="2" name="Tools"/>
-    <tableColumn id="3" name="GIT"/>
-    <tableColumn id="4" name="Atom"/>
-    <tableColumn id="5" name="Gantt Chart"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Person"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tools"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="GIT"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Atom"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Gantt Chart"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -952,27 +953,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="7"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="B1:BO30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B2" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B6" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" style="2" customWidth="1"/>
-    <col min="3" max="6" width="11.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15.6640625" style="4" customWidth="1"/>
-    <col min="8" max="27" width="2.77734375" style="1"/>
+    <col min="1" max="1" width="2.625" customWidth="1"/>
+    <col min="2" max="2" width="15.625" style="2" customWidth="1"/>
+    <col min="3" max="6" width="11.625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15.625" style="4" customWidth="1"/>
+    <col min="8" max="27" width="2.75" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:67" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="1.05">
+    <row r="1" spans="2:67" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
       <c r="B1" s="13" t="s">
         <v>0</v>
       </c>
@@ -982,14 +983,14 @@
       <c r="F1" s="12"/>
       <c r="G1" s="12"/>
     </row>
-    <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="20" t="s">
+    <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
       <c r="G2" s="5" t="s">
         <v>5</v>
       </c>
@@ -997,44 +998,44 @@
         <v>1</v>
       </c>
       <c r="J2" s="15"/>
-      <c r="K2" s="26" t="s">
+      <c r="K2" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
-      <c r="N2" s="27"/>
-      <c r="O2" s="27"/>
-      <c r="P2" s="27"/>
-      <c r="Q2" s="28"/>
+      <c r="L2" s="28"/>
+      <c r="M2" s="28"/>
+      <c r="N2" s="28"/>
+      <c r="O2" s="28"/>
+      <c r="P2" s="28"/>
+      <c r="Q2" s="29"/>
       <c r="R2" s="16"/>
-      <c r="S2" s="18" t="s">
+      <c r="S2" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="T2" s="19"/>
-      <c r="U2" s="19"/>
-      <c r="V2" s="19"/>
-      <c r="W2" s="19"/>
-      <c r="X2" s="19"/>
-      <c r="Y2" s="19"/>
-      <c r="Z2" s="19"/>
-    </row>
-    <row r="3" spans="2:67" s="11" customFormat="1" ht="39.9" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="21" t="s">
+      <c r="T2" s="20"/>
+      <c r="U2" s="20"/>
+      <c r="V2" s="20"/>
+      <c r="W2" s="20"/>
+      <c r="X2" s="20"/>
+      <c r="Y2" s="20"/>
+      <c r="Z2" s="20"/>
+    </row>
+    <row r="3" spans="2:67" s="11" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="23" t="s">
+      <c r="D3" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="23" t="s">
+      <c r="E3" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="23" t="s">
+      <c r="F3" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="25" t="s">
+      <c r="G3" s="26" t="s">
         <v>6</v>
       </c>
       <c r="H3" s="17" t="s">
@@ -1060,13 +1061,13 @@
       <c r="Z3" s="10"/>
       <c r="AA3" s="10"/>
     </row>
-    <row r="4" spans="2:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="22"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
+    <row r="4" spans="2:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="23"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
       <c r="H4" s="3">
         <v>1</v>
       </c>
@@ -1248,14 +1249,14 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="29">
+      <c r="C5" s="18">
         <v>42978</v>
       </c>
-      <c r="D5" s="29">
+      <c r="D5" s="18">
         <v>42999</v>
       </c>
       <c r="E5" s="7">
@@ -1268,14 +1269,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="29">
+      <c r="C6" s="18">
         <v>42978</v>
       </c>
-      <c r="D6" s="29">
+      <c r="D6" s="18">
         <v>42999</v>
       </c>
       <c r="E6" s="7">
@@ -1288,14 +1289,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="29">
+      <c r="C7" s="18">
         <v>42985</v>
       </c>
-      <c r="D7" s="29">
+      <c r="D7" s="18">
         <v>42999</v>
       </c>
       <c r="E7" s="7">
@@ -1308,14 +1309,14 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="8" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="29">
+      <c r="C8" s="18">
         <v>42999</v>
       </c>
-      <c r="D8" s="29">
+      <c r="D8" s="18">
         <v>43004</v>
       </c>
       <c r="E8" s="7">
@@ -1328,7 +1329,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="9" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9"/>
       <c r="C9"/>
       <c r="D9"/>
@@ -1356,7 +1357,7 @@
       <c r="Z9"/>
       <c r="AA9"/>
     </row>
-    <row r="10" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>8</v>
       </c>
@@ -1394,7 +1395,7 @@
       <c r="Z10"/>
       <c r="AA10"/>
     </row>
-    <row r="11" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>13</v>
       </c>
@@ -1432,14 +1433,22 @@
       <c r="Z11"/>
       <c r="AA11"/>
     </row>
-    <row r="12" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>14</v>
       </c>
-      <c r="C12"/>
-      <c r="D12"/>
-      <c r="E12"/>
-      <c r="F12"/>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>0.1</v>
+      </c>
       <c r="G12"/>
       <c r="H12"/>
       <c r="I12"/>
@@ -1462,14 +1471,22 @@
       <c r="Z12"/>
       <c r="AA12"/>
     </row>
-    <row r="13" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>15</v>
       </c>
-      <c r="C13"/>
-      <c r="D13"/>
-      <c r="E13"/>
-      <c r="F13"/>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0.1</v>
+      </c>
       <c r="G13"/>
       <c r="H13"/>
       <c r="I13"/>
@@ -1492,7 +1509,7 @@
       <c r="Z13"/>
       <c r="AA13"/>
     </row>
-    <row r="14" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>16</v>
       </c>
@@ -1522,14 +1539,22 @@
       <c r="Z14"/>
       <c r="AA14"/>
     </row>
-    <row r="15" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>17</v>
       </c>
-      <c r="C15"/>
-      <c r="D15"/>
-      <c r="E15"/>
-      <c r="F15"/>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
       <c r="G15"/>
       <c r="H15"/>
       <c r="I15"/>
@@ -1552,7 +1577,7 @@
       <c r="Z15"/>
       <c r="AA15"/>
     </row>
-    <row r="16" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="6"/>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
@@ -1580,7 +1605,7 @@
       <c r="Z16"/>
       <c r="AA16"/>
     </row>
-    <row r="17" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="6"/>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
@@ -1608,7 +1633,7 @@
       <c r="Z17"/>
       <c r="AA17"/>
     </row>
-    <row r="18" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="6"/>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
@@ -1636,7 +1661,7 @@
       <c r="Z18"/>
       <c r="AA18"/>
     </row>
-    <row r="19" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="6"/>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
@@ -1664,7 +1689,7 @@
       <c r="Z19"/>
       <c r="AA19"/>
     </row>
-    <row r="20" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="6"/>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
@@ -1692,7 +1717,7 @@
       <c r="Z20"/>
       <c r="AA20"/>
     </row>
-    <row r="21" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="6"/>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
@@ -1720,7 +1745,7 @@
       <c r="Z21"/>
       <c r="AA21"/>
     </row>
-    <row r="22" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="6"/>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
@@ -1748,7 +1773,7 @@
       <c r="Z22"/>
       <c r="AA22"/>
     </row>
-    <row r="23" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="6"/>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
@@ -1776,7 +1801,7 @@
       <c r="Z23"/>
       <c r="AA23"/>
     </row>
-    <row r="24" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="6"/>
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
@@ -1804,7 +1829,7 @@
       <c r="Z24"/>
       <c r="AA24"/>
     </row>
-    <row r="25" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="6"/>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
@@ -1832,7 +1857,7 @@
       <c r="Z25"/>
       <c r="AA25"/>
     </row>
-    <row r="26" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="6"/>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
@@ -1860,7 +1885,7 @@
       <c r="Z26"/>
       <c r="AA26"/>
     </row>
-    <row r="27" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="6"/>
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
@@ -1888,7 +1913,7 @@
       <c r="Z27"/>
       <c r="AA27"/>
     </row>
-    <row r="28" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="6"/>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
@@ -1916,7 +1941,7 @@
       <c r="Z28"/>
       <c r="AA28"/>
     </row>
-    <row r="29" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="6"/>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
@@ -1944,7 +1969,7 @@
       <c r="Z29"/>
       <c r="AA29"/>
     </row>
-    <row r="30" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="6"/>
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
@@ -2021,21 +2046,21 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="13">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Project planner uses periods for intervals. Start=1 is period 1 and duration=5 means project spans 5 periods starting from start period. Enter data starting in B5 to update the chart" sqref="A1"/>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Type a value from 1 to 60 or select a period from the list-press  CANCEL, ALT+DOWN ARROW, then ENTER to select a value" prompt="Enter a period in the range of 1 to 60 or select a period from the list. Press ALT+DOWN ARROW to navigate the list, then ENTER to select a value" sqref="H2">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Project planner uses periods for intervals. Start=1 is period 1 and duration=5 means project spans 5 periods starting from start period. Enter data starting in B5 to update the chart" sqref="A1" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Type a value from 1 to 60 or select a period from the list-press  CANCEL, ALT+DOWN ARROW, then ENTER to select a value" prompt="Enter a period in the range of 1 to 60 or select a period from the list. Press ALT+DOWN ARROW to navigate the list, then ENTER to select a value" sqref="H2" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16,17,18,19,20,21,22,23,24,25,26,27,28,29,30,31,32,33,34,35,36,37,38,39,40,41,42,43,44,45,46,47,48,49,50,51,52,53,54,55,56,57,58,59,60"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates actual duration beyond plan" sqref="J2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates the percentage of project completed beyond plan" sqref="R2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Periods are charted from 1 to 60 starting from cell H4 to cell BO4 " sqref="H3"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter activity in column B, starting with cell B5_x000a_" sqref="B3:B4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter plan start period in column C, starting with cell C5" sqref="C3:C4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter plan duration period in column D, starting with cell D5" sqref="D3:D4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter actual start period in column E, starting with cell E5" sqref="E3:E4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter actual duration period in column F, starting with cell F5" sqref="F3:F4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter the percentage of project completed in column G, starting with cell G5" sqref="G3:G4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Title of the project. Enter a new title in this cell. Highlight a period in H2. Chart legend is in J2 to AI2" sqref="B1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select a period to highlight in H2. A Chart legend is in J2 to AI2" sqref="B2:F2"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates actual duration beyond plan" sqref="J2" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates the percentage of project completed beyond plan" sqref="R2" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Periods are charted from 1 to 60 starting from cell H4 to cell BO4 " sqref="H3" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter activity in column B, starting with cell B5_x000a_" sqref="B3:B4" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter plan start period in column C, starting with cell C5" sqref="C3:C4" xr:uid="{00000000-0002-0000-0000-000006000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter plan duration period in column D, starting with cell D5" sqref="D3:D4" xr:uid="{00000000-0002-0000-0000-000007000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter actual start period in column E, starting with cell E5" sqref="E3:E4" xr:uid="{00000000-0002-0000-0000-000008000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter actual duration period in column F, starting with cell F5" sqref="F3:F4" xr:uid="{00000000-0002-0000-0000-000009000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter the percentage of project completed in column G, starting with cell G5" sqref="G3:G4" xr:uid="{00000000-0002-0000-0000-00000A000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Title of the project. Enter a new title in this cell. Highlight a period in H2. Chart legend is in J2 to AI2" sqref="B1" xr:uid="{00000000-0002-0000-0000-00000B000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select a period to highlight in H2. A Chart legend is in J2 to AI2" sqref="B2:F2" xr:uid="{00000000-0002-0000-0000-00000C000000}"/>
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.45" right="0.45" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>

</xml_diff>